<commit_message>
Got NTA code to run for the first time
</commit_message>
<xml_diff>
--- a/products analysis/reference compounds analysis/SCCPProdref list and analysis.xlsx
+++ b/products analysis/reference compounds analysis/SCCPProdref list and analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Steven\Target Decoy\products analysis\reference compounds analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C009A0A4-8638-4735-A5F4-70D1B40F6F71}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E57608-6FDD-4A02-B9EC-EBCCE91ECBD1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12870" yWindow="1140" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{1EB0EB00-CAC1-4803-AD13-83FA2283711D}"/>
+    <workbookView xWindow="6675" yWindow="270" windowWidth="21600" windowHeight="11385" xr2:uid="{1EB0EB00-CAC1-4803-AD13-83FA2283711D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample100" sheetId="1" r:id="rId1"/>
@@ -791,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F26ABEB-F7B0-4AE9-90A1-67889DFCE138}">
   <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:AB1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2246,8 +2246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55EA8B02-EDED-461E-9BCD-BF411E686BBD}">
   <dimension ref="A1:AE47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>